<commit_message>
completed 3 times docking
</commit_message>
<xml_diff>
--- a/vina/10-Ca1.3_ID_7UHG/active-site.xlsx
+++ b/vina/10-Ca1.3_ID_7UHG/active-site.xlsx
@@ -13,10 +13,10 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1682883495" val="1062" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1682883495" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1682883495"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1682883495"/>
+      <pm:revision xmlns:pm="smNativeData" day="1683037129" val="1062" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1683037129" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1683037129" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1683037129"/>
     </ext>
   </extLst>
 </workbook>
@@ -143,10 +143,10 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1682883495" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1683037129" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Times New Roman" sz="200" lang="default"/>
-            <pm:ea face="SimSun" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -158,7 +158,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1682883495" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1683037129" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -174,35 +174,24 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1682883495" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1683037129" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
-            <pm:cs face="Times New Roman" sz="200" lang="default"/>
-            <pm:ea face="SimSun" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default" weight="bold"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default" weight="bold"/>
           </pm:charSpec>
         </ext>
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1682883495" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -218,26 +207,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1682883495"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1682883495"/>
+          <pm:border xmlns:pm="smNativeData" id="1683037129"/>
         </ext>
       </extLst>
     </border>
@@ -245,16 +215,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,8 +228,8 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1682883495" count="1">
-        <pm:charStyle name="Normal" fontId="0"/>
+      <pm:charStyles xmlns:pm="smNativeData" id="1683037129" count="1">
+        <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
   </extLst>
@@ -322,8 +285,8 @@
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Arial"/>
-        <a:ea typeface="SimSun"/>
-        <a:cs typeface="Times New Roman"/>
+        <a:ea typeface="Basic Roman"/>
+        <a:cs typeface="Basic Roman"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,20 +494,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="B1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
+  <cols>
+    <col min="3" max="3" width="16.225225" customWidth="1"/>
+    <col min="4" max="4" width="15.828829" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:5">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -665,10 +632,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>157.705999999999989</v>
+        <v>157.70599999999996</v>
       </c>
       <c r="D10" t="n">
-        <v>146.389999999999986</v>
+        <v>146.389999999999958</v>
       </c>
       <c r="E10" t="n">
         <v>142.447000000000003</v>
@@ -708,30 +675,30 @@
       </c>
       <c r="C13">
         <f>AVERAGE(C2:C12)</f>
-        <v>154.779454545454513</v>
+        <v>154.779454545454996</v>
       </c>
       <c r="D13">
         <f>AVERAGE(D2:D12)</f>
-        <v>148.703181818181804</v>
+        <v>148.703181818182003</v>
       </c>
       <c r="E13">
         <f>AVERAGE(E2:E12)</f>
-        <v>144.321000000000026</v>
+        <v>144.320999999999998</v>
       </c>
     </row>
     <row r="15" spans="3:5">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="n">
@@ -745,7 +712,7 @@
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="n">
@@ -759,21 +726,21 @@
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="n">
         <v>143.424000000000007</v>
       </c>
       <c r="D18" t="n">
-        <v>157.877999999999986</v>
+        <v>157.877999999999957</v>
       </c>
       <c r="E18" t="n">
         <v>141.144000000000005</v>
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="n">
@@ -787,7 +754,7 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="n">
@@ -801,7 +768,7 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C21" t="n">
@@ -815,7 +782,7 @@
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" t="n">
@@ -825,11 +792,11 @@
         <v>155.746000000000009</v>
       </c>
       <c r="E22" t="n">
-        <v>153.776999999999987</v>
+        <v>153.776999999999958</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="n">
@@ -843,7 +810,7 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="n">
@@ -857,7 +824,7 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="n">
@@ -867,11 +834,11 @@
         <v>150.847000000000008</v>
       </c>
       <c r="E25" t="n">
-        <v>154.449999999999989</v>
+        <v>154.44999999999996</v>
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C26" t="n">
@@ -885,7 +852,7 @@
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C27" t="n">
@@ -904,26 +871,26 @@
       </c>
       <c r="C28">
         <f>AVERAGE(C16:C27)</f>
-        <v>144.512000000000029</v>
+        <v>144.512</v>
       </c>
       <c r="D28">
         <f>AVERAGE(D16:D27)</f>
-        <v>156.799500000000023</v>
+        <v>156.799499999999995</v>
       </c>
       <c r="E28">
         <f>AVERAGE(E16:E27)</f>
-        <v>150.98533333333333</v>
+        <v>150.985333333332989</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30"/>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -935,7 +902,7 @@
         <v>148.730999999999995</v>
       </c>
       <c r="D31" t="n">
-        <v>159.699999999999989</v>
+        <v>159.69999999999996</v>
       </c>
       <c r="E31" t="n">
         <v>139.268000000000001</v>
@@ -1017,22 +984,22 @@
       </c>
       <c r="C37">
         <f>AVERAGE(C31:C36)</f>
-        <v>151.869500000000016</v>
+        <v>151.869499999999988</v>
       </c>
       <c r="D37">
         <f>AVERAGE(D31:D36)</f>
-        <v>160.596166666666676</v>
+        <v>160.596166666666988</v>
       </c>
       <c r="E37">
         <f>AVERAGE(E31:E36)</f>
-        <v>140.951833333333354</v>
+        <v>140.951833333333013</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1682883495" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1683037129" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1041,14 +1008,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1682883495" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1682883495" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1683037129" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1683037129" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1682883495" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1683037129" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>